<commit_message>
perf tests for graph are rewritten to have one class
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it-performance/src/test/resources/datamodel/graph/SIMPLE_100times.xlsx
+++ b/calculation-engine/engine-tests/engine-it-performance/src/test/resources/datamodel/graph/SIMPLE_100times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1005" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1455" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -358,8 +358,8 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
-        <f>B1*C1+SUM(D1,E1,F1)/G1-H1</f>
-        <v>2</v>
+        <f>B1*C1+SUM(D1,E1,F1)/G1-H1+526</f>
+        <v>528</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -385,8 +385,8 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f t="shared" ref="A2:A65" si="0">B2*C2+SUM(D2,E2,F2)/G2-H2</f>
-        <v>2</v>
+        <f t="shared" ref="A2:A65" si="0">B2*C2+SUM(D2,E2,F2)/G2-H2+526</f>
+        <v>528</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -413,7 +413,7 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -440,7 +440,7 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -467,7 +467,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -494,7 +494,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -521,7 +521,7 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -548,7 +548,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -575,7 +575,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -602,7 +602,7 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -629,7 +629,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -656,7 +656,7 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -683,7 +683,7 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -710,7 +710,7 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -737,7 +737,7 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -764,7 +764,7 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -791,7 +791,7 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -818,7 +818,7 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -845,7 +845,7 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -872,7 +872,7 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -899,7 +899,7 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -926,7 +926,7 @@
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -953,7 +953,7 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -980,7 +980,7 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1007,7 +1007,7 @@
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1034,7 +1034,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1061,7 +1061,7 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1088,7 +1088,7 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1115,7 +1115,7 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1142,7 +1142,7 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1169,7 +1169,7 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1196,7 +1196,7 @@
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1223,7 +1223,7 @@
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1250,7 +1250,7 @@
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1277,7 +1277,7 @@
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1304,7 +1304,7 @@
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -1331,7 +1331,7 @@
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1358,7 +1358,7 @@
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1385,7 +1385,7 @@
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -1412,7 +1412,7 @@
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -1439,7 +1439,7 @@
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -1466,7 +1466,7 @@
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -1493,7 +1493,7 @@
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -1520,7 +1520,7 @@
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -1547,7 +1547,7 @@
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -1574,7 +1574,7 @@
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -1601,7 +1601,7 @@
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -1628,7 +1628,7 @@
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -1655,7 +1655,7 @@
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -1682,7 +1682,7 @@
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -1709,7 +1709,7 @@
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -1736,7 +1736,7 @@
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -1763,7 +1763,7 @@
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -1790,7 +1790,7 @@
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -1817,7 +1817,7 @@
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -1844,7 +1844,7 @@
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -1871,7 +1871,7 @@
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -1898,7 +1898,7 @@
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -1925,7 +1925,7 @@
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -1952,7 +1952,7 @@
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -1979,7 +1979,7 @@
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -2006,7 +2006,7 @@
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -2033,7 +2033,7 @@
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -2060,7 +2060,7 @@
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -2087,7 +2087,7 @@
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -2113,8 +2113,8 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f t="shared" ref="A66:A100" si="1">B66*C66+SUM(D66,E66,F66)/G66-H66</f>
-        <v>2</v>
+        <f t="shared" ref="A66:A100" si="1">B66*C66+SUM(D66,E66,F66)/G66-H66+526</f>
+        <v>528</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -2141,7 +2141,7 @@
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -2168,7 +2168,7 @@
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -2195,7 +2195,7 @@
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2222,7 +2222,7 @@
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2249,7 +2249,7 @@
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2276,7 +2276,7 @@
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2303,7 +2303,7 @@
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2330,7 +2330,7 @@
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2357,7 +2357,7 @@
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2384,7 +2384,7 @@
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2411,7 +2411,7 @@
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -2438,7 +2438,7 @@
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -2465,7 +2465,7 @@
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -2492,7 +2492,7 @@
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -2519,7 +2519,7 @@
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -2546,7 +2546,7 @@
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B82">
         <v>1</v>
@@ -2573,7 +2573,7 @@
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -2600,7 +2600,7 @@
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -2627,7 +2627,7 @@
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -2654,7 +2654,7 @@
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -2681,7 +2681,7 @@
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -2708,7 +2708,7 @@
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2735,7 +2735,7 @@
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -2762,7 +2762,7 @@
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -2789,7 +2789,7 @@
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2816,7 +2816,7 @@
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -2843,7 +2843,7 @@
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -2870,7 +2870,7 @@
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -2897,7 +2897,7 @@
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -2924,7 +2924,7 @@
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -2951,7 +2951,7 @@
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -2978,7 +2978,7 @@
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -3005,7 +3005,7 @@
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -3032,7 +3032,7 @@
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="B100">
         <v>1</v>

</xml_diff>